<commit_message>
Updating the Time Sheet
</commit_message>
<xml_diff>
--- a/TimeTracking.xlsx
+++ b/TimeTracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver\Documents\School\CapStoneProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silva\Desktop\ProjectStone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -557,9 +557,12 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
       <c r="C6">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <f>D6+E5</f>
@@ -580,10 +583,10 @@
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E5:E13" si="3">D7+E6</f>
+        <f t="shared" ref="E7:E13" si="3">D7+E6</f>
         <v>20</v>
       </c>
       <c r="G7">
@@ -601,7 +604,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
@@ -622,7 +625,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
@@ -643,7 +646,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
@@ -664,7 +667,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
@@ -685,7 +688,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
@@ -706,7 +709,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Saving because we are about merge for our alpha
</commit_message>
<xml_diff>
--- a/TimeTracking.xlsx
+++ b/TimeTracking.xlsx
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -656,42 +656,66 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>74</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>70</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G7:G13" si="2">F9</f>
-        <v>0</v>
+        <f>F9+G8</f>
+        <v>66</v>
+      </c>
+      <c r="H9">
+        <v>11</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I7:I13" si="3">H9</f>
-        <v>0</v>
+        <f>H9+I8</f>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>86</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="F10">
+        <v>11</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>F10+G9</f>
+        <v>77</v>
+      </c>
+      <c r="H10">
+        <v>13</v>
       </c>
       <c r="I10">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>H10+I9</f>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -700,18 +724,18 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G9:G13" si="2">F11</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I9:I13" si="3">H11</f>
         <v>0</v>
       </c>
     </row>
@@ -721,11 +745,11 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
@@ -742,11 +766,11 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
last couple of commits
</commit_message>
<xml_diff>
--- a/TimeTracking.xlsx
+++ b/TimeTracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -432,7 +432,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -731,11 +731,11 @@
         <v>84</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G9:G13" si="2">F11</f>
+        <f t="shared" ref="G11:G13" si="2">F11</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I9:I13" si="3">H11</f>
+        <f t="shared" ref="I11:I13" si="3">H11</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>